<commit_message>
Data feed works fine, though the regions are not sliced but added as one vector, which seems to be adequat enough for first diagnostics.
</commit_message>
<xml_diff>
--- a/Settings/datafeeds_settings/WSA_settings.xlsx
+++ b/Settings/datafeeds_settings/WSA_settings.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
   <si>
     <t>Ingots</t>
   </si>
@@ -122,7 +123,67 @@
     <t>WSABOFsteel</t>
   </si>
   <si>
-    <t>datafeed_name</t>
+    <t>WSAEAFsteel</t>
+  </si>
+  <si>
+    <t>FeedName</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>43-58</t>
+  </si>
+  <si>
+    <t>45-125</t>
+  </si>
+  <si>
+    <t>WSAFlatRolledProducts</t>
+  </si>
+  <si>
+    <t>[33-42,59-63]</t>
+  </si>
+  <si>
+    <t>126-231</t>
+  </si>
+  <si>
+    <t>WSALongRolledProducts</t>
+  </si>
+  <si>
+    <t>WSAIngots</t>
+  </si>
+  <si>
+    <t>25-27</t>
+  </si>
+  <si>
+    <t>35-38</t>
+  </si>
+  <si>
+    <t>WSAOHFsteel</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>11-13</t>
+  </si>
+  <si>
+    <t>WSAPigIron</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>7-10</t>
+  </si>
+  <si>
+    <t>WSASpongeIron</t>
   </si>
 </sst>
 </file>
@@ -158,8 +219,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,82 +502,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.90625" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -525,177 +625,495 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D7:E7" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A few new data feed settings added.
</commit_message>
<xml_diff>
--- a/Settings/datafeeds_settings/WSA_settings.xlsx
+++ b/Settings/datafeeds_settings/WSA_settings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
   <si>
     <t>Ingots</t>
   </si>
@@ -63,9 +63,6 @@
     <t>TotalProductionOfCrudeSteel</t>
   </si>
   <si>
-    <t>RailwayTrackMaterial</t>
-  </si>
-  <si>
     <t>HeavySections</t>
   </si>
   <si>
@@ -184,6 +181,42 @@
   </si>
   <si>
     <t>WSASpongeIron</t>
+  </si>
+  <si>
+    <t>WSACrudeSteel</t>
+  </si>
+  <si>
+    <t>35-44</t>
+  </si>
+  <si>
+    <t>25-32</t>
+  </si>
+  <si>
+    <t>39-44</t>
+  </si>
+  <si>
+    <t>28-32</t>
+  </si>
+  <si>
+    <t>WSALiquidSteelForCastings</t>
+  </si>
+  <si>
+    <t>WSAContinuouslyCastSteel</t>
+  </si>
+  <si>
+    <t>20-24</t>
+  </si>
+  <si>
+    <t>30-34</t>
+  </si>
+  <si>
+    <t>WSAHotRolledProducts</t>
+  </si>
+  <si>
+    <t>45-231</t>
+  </si>
+  <si>
+    <t>33-63</t>
   </si>
 </sst>
 </file>
@@ -502,35 +535,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="31.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -541,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1">
         <v>20</v>
@@ -558,7 +591,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1">
         <v>22</v>
@@ -575,13 +608,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -592,13 +625,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -609,13 +642,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -626,13 +659,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -643,13 +676,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -660,14 +693,86 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="D10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14"/>
+      <c r="C14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -680,199 +785,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A8:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="42.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -880,16 +856,16 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -897,16 +873,16 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -914,16 +890,16 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -931,16 +907,16 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -948,16 +924,16 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -965,16 +941,16 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -982,16 +958,16 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -999,16 +975,16 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1016,16 +992,16 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1033,16 +1009,16 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1050,16 +1026,16 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1067,16 +1043,16 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1084,16 +1060,16 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1101,16 +1077,16 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restructured the folders in settings and concordances. One data feed creates problems, testing underway.
</commit_message>
<xml_diff>
--- a/Settings/datafeeds_settings/WSA_settings.xlsx
+++ b/Settings/datafeeds_settings/WSA_settings.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" r:id="rId1"/>
-    <sheet name="S2R" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>Ingots</t>
   </si>
@@ -235,34 +234,14 @@
   </si>
   <si>
     <t>SteelOpenHearthFurnace</t>
-  </si>
-  <si>
-    <t>aggregator</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>industry</t>
-  </si>
-  <si>
-    <t>product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -290,12 +269,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1029,43 +1007,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2">
-        <v>20200421</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3">
-        <v>20200421</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>